<commit_message>
2024.07.12 1) Create a Log Field (Time + Response Hex Data) 2) Store a query response data in 14-digit increments 3) Store 14 digits of data in each dictionary inside the constant file
</commit_message>
<xml_diff>
--- a/Command/Command.xlsx
+++ b/Command/Command.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Project\Python\TestTool\Command\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14C2BF7-8EDF-459E-9B79-EA790B4160BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCC174B-6B74-41D6-AA27-43811FD50FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{79FED000-970D-0E48-B65E-FB5160DD82FF}"/>
+    <workbookView xWindow="31350" yWindow="2880" windowWidth="21600" windowHeight="11295" xr2:uid="{79FED000-970D-0E48-B65E-FB5160DD82FF}"/>
   </bookViews>
   <sheets>
     <sheet name="IR RAW CMD" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="161">
   <si>
     <r>
       <rPr>
@@ -707,6 +707,26 @@
   </si>
   <si>
     <t>Cali. Interval 180</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Image Query</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cali. Query</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ETC Query</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status Query</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version Query</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -788,7 +808,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1053,21 +1073,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -1125,6 +1130,240 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1132,7 +1371,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1300,9 +1539,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1315,7 +1551,73 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1966,13 +2268,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2191A3BB-5475-EC49-9D9F-17B4E3E33BE8}">
-  <dimension ref="B1:W91"/>
+  <dimension ref="B1:W94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="J81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="M98" sqref="M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2001,78 +2303,78 @@
       </c>
     </row>
     <row r="2" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="59" t="s">
+      <c r="B2" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="59" t="s">
+      <c r="H2" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="59" t="s">
+      <c r="I2" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="59" t="s">
+      <c r="J2" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="59" t="s">
+      <c r="K2" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="59" t="s">
+      <c r="L2" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="59" t="s">
+      <c r="M2" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="59" t="s">
+      <c r="N2" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="60" t="s">
+      <c r="O2" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="61" t="s">
+      <c r="P2" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="61" t="s">
+      <c r="Q2" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="61" t="s">
+      <c r="R2" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="61" t="s">
+      <c r="S2" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="61" t="s">
+      <c r="T2" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="61" t="s">
+      <c r="U2" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="61" t="s">
+      <c r="V2" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="W2" s="62" t="s">
+      <c r="W2" s="60" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="70"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
@@ -2134,10 +2436,10 @@
       </c>
     </row>
     <row r="4" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="71"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -2199,10 +2501,10 @@
       </c>
     </row>
     <row r="5" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="32"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="32"/>
       <c r="E5" s="32"/>
       <c r="F5" s="32"/>
@@ -2263,10 +2565,10 @@
       </c>
     </row>
     <row r="6" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
@@ -2328,10 +2630,10 @@
       </c>
     </row>
     <row r="7" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -2393,10 +2695,10 @@
       </c>
     </row>
     <row r="8" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -2458,10 +2760,10 @@
       </c>
     </row>
     <row r="9" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -2523,10 +2825,10 @@
       </c>
     </row>
     <row r="10" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -2588,10 +2890,10 @@
       </c>
     </row>
     <row r="11" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -2653,10 +2955,10 @@
       </c>
     </row>
     <row r="12" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="71"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -2718,10 +3020,10 @@
       </c>
     </row>
     <row r="13" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="71"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -2783,10 +3085,10 @@
       </c>
     </row>
     <row r="14" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="71"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -2848,10 +3150,10 @@
       </c>
     </row>
     <row r="15" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2870,15 +3172,15 @@
         <v>16</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="N15" s="3" t="str">
         <f t="shared" si="46"/>
-        <v>5B</v>
+        <v>57</v>
       </c>
       <c r="O15" s="12" t="str">
         <f t="shared" ref="O15:O16" si="57">"FF01"&amp;J15&amp;""&amp;K15&amp;L15&amp;M15&amp;N15</f>
-        <v>FF01015500045B</v>
+        <v>FF010155000057</v>
       </c>
       <c r="P15" s="14" t="s">
         <v>9</v>
@@ -2901,22 +3203,22 @@
       </c>
       <c r="U15" s="15">
         <f t="shared" ref="U15:U16" si="62">HEX2DEC(M15)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V15" s="15">
         <f t="shared" ref="V15:V16" si="63">SUM(Q15:U15)</f>
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="W15" s="30" t="str">
         <f t="shared" ref="W15:W16" si="64">REPT("0",2-LEN(RIGHT(DEC2HEX(V15), 2)))&amp;RIGHT(DEC2HEX(V15), 2)</f>
-        <v>5B</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2978,10 +3280,10 @@
       </c>
     </row>
     <row r="17" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="32"/>
+      <c r="C17" s="72"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
@@ -3043,10 +3345,10 @@
       </c>
     </row>
     <row r="18" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="80" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
@@ -3108,10 +3410,10 @@
       </c>
     </row>
     <row r="19" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="71"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -3173,10 +3475,10 @@
       </c>
     </row>
     <row r="20" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="71"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -3238,10 +3540,10 @@
       </c>
     </row>
     <row r="21" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="71"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -3303,10 +3605,10 @@
       </c>
     </row>
     <row r="22" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="71"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -3368,10 +3670,10 @@
       </c>
     </row>
     <row r="23" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="71"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -3433,10 +3735,10 @@
       </c>
     </row>
     <row r="24" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="71"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -3498,10 +3800,10 @@
       </c>
     </row>
     <row r="25" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="71"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -3563,10 +3865,10 @@
       </c>
     </row>
     <row r="26" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="71"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -3628,10 +3930,10 @@
       </c>
     </row>
     <row r="27" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="71"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -3693,10 +3995,10 @@
       </c>
     </row>
     <row r="28" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="71"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -3758,10 +4060,10 @@
       </c>
     </row>
     <row r="29" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="3"/>
+      <c r="C29" s="71"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -3823,10 +4125,10 @@
       </c>
     </row>
     <row r="30" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="71"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -3848,7 +4150,7 @@
         <v>9</v>
       </c>
       <c r="N30" s="3" t="str">
-        <f t="shared" ref="N30:N31" si="92">W30</f>
+        <f t="shared" ref="N30:N33" si="92">W30</f>
         <v>B5</v>
       </c>
       <c r="O30" s="12" t="str">
@@ -3888,10 +4190,10 @@
       </c>
     </row>
     <row r="31" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="71"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -3953,10 +4255,10 @@
       </c>
     </row>
     <row r="32" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="78" t="s">
         <v>130</v>
       </c>
-      <c r="C32" s="32"/>
+      <c r="C32" s="72"/>
       <c r="D32" s="32"/>
       <c r="E32" s="32"/>
       <c r="F32" s="32"/>
@@ -4018,10 +4320,10 @@
       </c>
     </row>
     <row r="33" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="80" t="s">
         <v>134</v>
       </c>
-      <c r="C33" s="22"/>
+      <c r="C33" s="70"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
@@ -4042,19 +4344,19 @@
       <c r="M33" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="N33" s="24" t="s">
-        <v>16</v>
+      <c r="N33" s="3" t="str">
+        <f t="shared" si="92"/>
+        <v>A2</v>
       </c>
       <c r="O33" s="25" t="str">
         <f>"FF01"&amp;J33&amp;""&amp;K33&amp;L33&amp;M33&amp;N33</f>
-        <v>FF01A100000000</v>
+        <v>FF01A1000000A2</v>
       </c>
       <c r="P33" s="26" t="s">
         <v>9</v>
       </c>
       <c r="Q33" s="27">
-        <f>HEX2DEC(I33)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33" s="27">
         <f>HEX2DEC(J33)</f>
@@ -4074,18 +4376,18 @@
       </c>
       <c r="V33" s="27">
         <f>SUM(Q33:U33)</f>
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="W33" s="28" t="str">
         <f>REPT("0",2-LEN(RIGHT(DEC2HEX(V33), 2)))&amp;RIGHT(DEC2HEX(V33), 2)</f>
-        <v>A1</v>
+        <v>A2</v>
       </c>
     </row>
     <row r="34" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="3"/>
+      <c r="C34" s="71"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -4147,10 +4449,10 @@
       </c>
     </row>
     <row r="35" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="3"/>
+      <c r="C35" s="71"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -4212,10 +4514,10 @@
       </c>
     </row>
     <row r="36" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="3"/>
+      <c r="C36" s="71"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -4277,10 +4579,10 @@
       </c>
     </row>
     <row r="37" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="3"/>
+      <c r="C37" s="71"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -4342,10 +4644,10 @@
       </c>
     </row>
     <row r="38" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="3"/>
+      <c r="C38" s="71"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -4407,10 +4709,10 @@
       </c>
     </row>
     <row r="39" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="3"/>
+      <c r="C39" s="71"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -4472,10 +4774,10 @@
       </c>
     </row>
     <row r="40" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="3"/>
+      <c r="C40" s="71"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -4537,10 +4839,10 @@
       </c>
     </row>
     <row r="41" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="3"/>
+      <c r="C41" s="71"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -4602,10 +4904,10 @@
       </c>
     </row>
     <row r="42" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="3"/>
+      <c r="C42" s="71"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -4667,10 +4969,10 @@
       </c>
     </row>
     <row r="43" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="3"/>
+      <c r="C43" s="71"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -4732,10 +5034,10 @@
       </c>
     </row>
     <row r="44" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="3"/>
+      <c r="C44" s="71"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -4797,10 +5099,10 @@
       </c>
     </row>
     <row r="45" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="77" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="3"/>
+      <c r="C45" s="71"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -4862,10 +5164,10 @@
       </c>
     </row>
     <row r="46" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="3"/>
+      <c r="C46" s="71"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -4927,10 +5229,10 @@
       </c>
     </row>
     <row r="47" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="3"/>
+      <c r="C47" s="71"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -4992,10 +5294,10 @@
       </c>
     </row>
     <row r="48" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="3"/>
+      <c r="C48" s="71"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -5057,10 +5359,10 @@
       </c>
     </row>
     <row r="49" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="3"/>
+      <c r="C49" s="71"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -5122,10 +5424,10 @@
       </c>
     </row>
     <row r="50" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="C50" s="3"/>
+      <c r="C50" s="71"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -5187,10 +5489,10 @@
       </c>
     </row>
     <row r="51" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="32"/>
+      <c r="C51" s="72"/>
       <c r="D51" s="32"/>
       <c r="E51" s="32"/>
       <c r="F51" s="32"/>
@@ -5252,10 +5554,10 @@
       </c>
     </row>
     <row r="52" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="C52" s="22"/>
+      <c r="B52" s="80" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="70"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
@@ -5317,10 +5619,10 @@
       </c>
     </row>
     <row r="53" spans="2:23" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="3"/>
+      <c r="C53" s="71"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -5382,10 +5684,10 @@
       </c>
     </row>
     <row r="54" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="3"/>
+      <c r="C54" s="71"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -5447,10 +5749,10 @@
       </c>
     </row>
     <row r="55" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="C55" s="3"/>
+      <c r="C55" s="71"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -5512,10 +5814,10 @@
       </c>
     </row>
     <row r="56" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="29" t="s">
+      <c r="B56" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="3"/>
+      <c r="C56" s="71"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -5577,10 +5879,10 @@
       </c>
     </row>
     <row r="57" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="3"/>
+      <c r="C57" s="71"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -5642,10 +5944,10 @@
       </c>
     </row>
     <row r="58" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="3"/>
+      <c r="C58" s="71"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -5707,10 +6009,10 @@
       </c>
     </row>
     <row r="59" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="29" t="s">
+      <c r="B59" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="3"/>
+      <c r="C59" s="71"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -5772,10 +6074,10 @@
       </c>
     </row>
     <row r="60" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="29" t="s">
+      <c r="B60" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C60" s="3"/>
+      <c r="C60" s="71"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -5837,10 +6139,10 @@
       </c>
     </row>
     <row r="61" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="29" t="s">
+      <c r="B61" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="C61" s="3"/>
+      <c r="C61" s="71"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -5902,10 +6204,10 @@
       </c>
     </row>
     <row r="62" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="29" t="s">
+      <c r="B62" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="C62" s="3"/>
+      <c r="C62" s="71"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -5967,10 +6269,10 @@
       </c>
     </row>
     <row r="63" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="29" t="s">
+      <c r="B63" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="3"/>
+      <c r="C63" s="71"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -6032,10 +6334,10 @@
       </c>
     </row>
     <row r="64" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="29" t="s">
+      <c r="B64" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="C64" s="3"/>
+      <c r="C64" s="71"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -6097,10 +6399,10 @@
       </c>
     </row>
     <row r="65" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="29" t="s">
+      <c r="B65" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="C65" s="3"/>
+      <c r="C65" s="71"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -6162,10 +6464,10 @@
       </c>
     </row>
     <row r="66" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="29" t="s">
+      <c r="B66" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C66" s="3"/>
+      <c r="C66" s="71"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -6227,10 +6529,10 @@
       </c>
     </row>
     <row r="67" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="29" t="s">
+      <c r="B67" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C67" s="3"/>
+      <c r="C67" s="71"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -6292,10 +6594,10 @@
       </c>
     </row>
     <row r="68" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="31" t="s">
+      <c r="B68" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="C68" s="32"/>
+      <c r="C68" s="72"/>
       <c r="D68" s="32"/>
       <c r="E68" s="32"/>
       <c r="F68" s="32"/>
@@ -6357,75 +6659,75 @@
       </c>
     </row>
     <row r="69" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="40" t="s">
+      <c r="B69" s="80" t="s">
         <v>135</v>
       </c>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J69" s="3" t="s">
+      <c r="C69" s="70"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="23"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J69" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="K69" s="3">
+      <c r="K69" s="22">
         <v>30</v>
       </c>
-      <c r="L69" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N69" s="3" t="str">
+      <c r="L69" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M69" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="N69" s="22" t="str">
         <f t="shared" ref="N69:N84" si="222">W69</f>
         <v>D2</v>
       </c>
-      <c r="O69" s="12" t="str">
+      <c r="O69" s="25" t="str">
         <f t="shared" ref="O69:O84" si="223">"FF01"&amp;J69&amp;""&amp;K69&amp;L69&amp;M69&amp;N69</f>
         <v>FF01A1300000D2</v>
       </c>
-      <c r="P69" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q69" s="15">
+      <c r="P69" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q69" s="27">
         <f t="shared" ref="Q69:Q84" si="224">HEX2DEC(I69)</f>
         <v>1</v>
       </c>
-      <c r="R69" s="15">
+      <c r="R69" s="27">
         <f t="shared" ref="R69:R84" si="225">HEX2DEC(J69)</f>
         <v>161</v>
       </c>
-      <c r="S69" s="15">
+      <c r="S69" s="27">
         <f t="shared" ref="S69:S84" si="226">HEX2DEC(K69)</f>
         <v>48</v>
       </c>
-      <c r="T69" s="15">
+      <c r="T69" s="27">
         <f t="shared" ref="T69:T84" si="227">HEX2DEC(L69)</f>
         <v>0</v>
       </c>
-      <c r="U69" s="15">
+      <c r="U69" s="27">
         <f t="shared" ref="U69:U84" si="228">HEX2DEC(M69)</f>
         <v>0</v>
       </c>
-      <c r="V69" s="15">
+      <c r="V69" s="27">
         <f t="shared" ref="V69:V84" si="229">SUM(Q69:U69)</f>
         <v>210</v>
       </c>
-      <c r="W69" s="15" t="str">
+      <c r="W69" s="28" t="str">
         <f t="shared" ref="W69:W91" si="230">REPT("0",2-LEN(RIGHT(DEC2HEX(V69), 2)))&amp;RIGHT(DEC2HEX(V69), 2)</f>
         <v>D2</v>
       </c>
     </row>
     <row r="70" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="C70" s="3"/>
+      <c r="C70" s="71"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -6481,16 +6783,16 @@
         <f t="shared" si="229"/>
         <v>210</v>
       </c>
-      <c r="W70" s="15" t="str">
+      <c r="W70" s="30" t="str">
         <f t="shared" si="230"/>
         <v>D2</v>
       </c>
     </row>
     <row r="71" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="77" t="s">
         <v>137</v>
       </c>
-      <c r="C71" s="3"/>
+      <c r="C71" s="71"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -6546,16 +6848,16 @@
         <f t="shared" si="229"/>
         <v>211</v>
       </c>
-      <c r="W71" s="15" t="str">
+      <c r="W71" s="30" t="str">
         <f t="shared" si="230"/>
         <v>D3</v>
       </c>
     </row>
     <row r="72" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="77" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="3"/>
+      <c r="C72" s="71"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -6611,16 +6913,16 @@
         <f t="shared" si="229"/>
         <v>211</v>
       </c>
-      <c r="W72" s="15" t="str">
+      <c r="W72" s="30" t="str">
         <f t="shared" si="230"/>
         <v>D3</v>
       </c>
     </row>
     <row r="73" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="77" t="s">
         <v>139</v>
       </c>
-      <c r="C73" s="3"/>
+      <c r="C73" s="71"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -6676,16 +6978,16 @@
         <f t="shared" si="229"/>
         <v>251</v>
       </c>
-      <c r="W73" s="15" t="str">
+      <c r="W73" s="30" t="str">
         <f t="shared" si="230"/>
         <v>FB</v>
       </c>
     </row>
     <row r="74" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="77" t="s">
         <v>141</v>
       </c>
-      <c r="C74" s="3"/>
+      <c r="C74" s="71"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -6741,16 +7043,16 @@
         <f t="shared" si="229"/>
         <v>212</v>
       </c>
-      <c r="W74" s="15" t="str">
+      <c r="W74" s="30" t="str">
         <f t="shared" si="230"/>
         <v>D4</v>
       </c>
     </row>
     <row r="75" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="77" t="s">
         <v>142</v>
       </c>
-      <c r="C75" s="3"/>
+      <c r="C75" s="71"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
@@ -6806,16 +7108,16 @@
         <f t="shared" si="229"/>
         <v>252</v>
       </c>
-      <c r="W75" s="15" t="str">
+      <c r="W75" s="30" t="str">
         <f t="shared" si="230"/>
         <v>FC</v>
       </c>
     </row>
     <row r="76" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="77" t="s">
         <v>143</v>
       </c>
-      <c r="C76" s="3"/>
+      <c r="C76" s="71"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -6871,16 +7173,16 @@
         <f t="shared" si="229"/>
         <v>213</v>
       </c>
-      <c r="W76" s="15" t="str">
+      <c r="W76" s="30" t="str">
         <f t="shared" si="230"/>
         <v>D5</v>
       </c>
     </row>
     <row r="77" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="C77" s="3"/>
+      <c r="C77" s="71"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
@@ -6936,16 +7238,16 @@
         <f t="shared" si="229"/>
         <v>214</v>
       </c>
-      <c r="W77" s="15" t="str">
+      <c r="W77" s="30" t="str">
         <f t="shared" si="230"/>
         <v>D6</v>
       </c>
     </row>
     <row r="78" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="C78" s="3"/>
+      <c r="C78" s="71"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
@@ -7001,16 +7303,16 @@
         <f t="shared" si="229"/>
         <v>214</v>
       </c>
-      <c r="W78" s="15" t="str">
+      <c r="W78" s="30" t="str">
         <f t="shared" si="230"/>
         <v>D6</v>
       </c>
     </row>
     <row r="79" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C79" s="3"/>
+      <c r="C79" s="71"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
@@ -7066,16 +7368,16 @@
         <f t="shared" si="229"/>
         <v>215</v>
       </c>
-      <c r="W79" s="15" t="str">
+      <c r="W79" s="30" t="str">
         <f t="shared" si="230"/>
         <v>D7</v>
       </c>
     </row>
     <row r="80" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="C80" s="16"/>
+      <c r="C80" s="73"/>
       <c r="D80" s="16"/>
       <c r="E80" s="16"/>
       <c r="F80" s="16"/>
@@ -7131,16 +7433,16 @@
         <f t="shared" si="229"/>
         <v>216</v>
       </c>
-      <c r="W80" s="21" t="str">
+      <c r="W80" s="61" t="str">
         <f t="shared" si="230"/>
         <v>D8</v>
       </c>
     </row>
     <row r="81" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="C81" s="16"/>
+      <c r="C81" s="73"/>
       <c r="D81" s="16"/>
       <c r="E81" s="16"/>
       <c r="F81" s="16"/>
@@ -7196,16 +7498,16 @@
         <f t="shared" si="229"/>
         <v>215</v>
       </c>
-      <c r="W81" s="21" t="str">
+      <c r="W81" s="61" t="str">
         <f t="shared" si="230"/>
         <v>D7</v>
       </c>
     </row>
     <row r="82" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="16" t="s">
+      <c r="B82" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="C82" s="16"/>
+      <c r="C82" s="73"/>
       <c r="D82" s="16"/>
       <c r="E82" s="16"/>
       <c r="F82" s="16"/>
@@ -7261,16 +7563,16 @@
         <f t="shared" si="229"/>
         <v>216</v>
       </c>
-      <c r="W82" s="21" t="str">
+      <c r="W82" s="61" t="str">
         <f t="shared" si="230"/>
         <v>D8</v>
       </c>
     </row>
     <row r="83" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="16" t="s">
+      <c r="B83" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="C83" s="16"/>
+      <c r="C83" s="73"/>
       <c r="D83" s="16"/>
       <c r="E83" s="16"/>
       <c r="F83" s="16"/>
@@ -7326,146 +7628,146 @@
         <f t="shared" si="229"/>
         <v>217</v>
       </c>
-      <c r="W83" s="21" t="str">
+      <c r="W83" s="61" t="str">
         <f t="shared" si="230"/>
         <v>D9</v>
       </c>
     </row>
-    <row r="84" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="16" t="s">
+    <row r="84" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B84" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="C84" s="16"/>
-      <c r="D84" s="16"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="16"/>
-      <c r="I84" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="J84" s="16" t="s">
+      <c r="C84" s="72"/>
+      <c r="D84" s="32"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="32"/>
+      <c r="G84" s="33"/>
+      <c r="H84" s="32"/>
+      <c r="I84" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="J84" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="K84" s="16">
+      <c r="K84" s="32">
         <v>36</v>
       </c>
-      <c r="L84" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="M84" s="18" t="s">
+      <c r="L84" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="M84" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="N84" s="16" t="str">
+      <c r="N84" s="32" t="str">
         <f t="shared" si="222"/>
         <v>DA</v>
       </c>
-      <c r="O84" s="19" t="str">
+      <c r="O84" s="35" t="str">
         <f t="shared" si="223"/>
         <v>FF01A0360003DA</v>
       </c>
-      <c r="P84" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q84" s="21">
+      <c r="P84" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q84" s="37">
         <f t="shared" si="224"/>
         <v>1</v>
       </c>
-      <c r="R84" s="21">
+      <c r="R84" s="37">
         <f t="shared" si="225"/>
         <v>160</v>
       </c>
-      <c r="S84" s="21">
+      <c r="S84" s="37">
         <f t="shared" si="226"/>
         <v>54</v>
       </c>
-      <c r="T84" s="21">
+      <c r="T84" s="37">
         <f t="shared" si="227"/>
         <v>0</v>
       </c>
-      <c r="U84" s="21">
+      <c r="U84" s="37">
         <f t="shared" si="228"/>
         <v>3</v>
       </c>
-      <c r="V84" s="21">
+      <c r="V84" s="37">
         <f t="shared" si="229"/>
         <v>218</v>
       </c>
-      <c r="W84" s="21" t="str">
+      <c r="W84" s="38" t="str">
         <f t="shared" si="230"/>
         <v>DA</v>
       </c>
     </row>
     <row r="85" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C85" s="16"/>
-      <c r="D85" s="16"/>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="16"/>
-      <c r="I85" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="J85" s="16" t="s">
+      <c r="B85" s="82" t="s">
+        <v>157</v>
+      </c>
+      <c r="C85" s="74"/>
+      <c r="D85" s="62"/>
+      <c r="E85" s="62"/>
+      <c r="F85" s="62"/>
+      <c r="G85" s="63"/>
+      <c r="H85" s="62"/>
+      <c r="I85" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="J85" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="K85" s="16">
+      <c r="K85" s="62">
         <v>40</v>
       </c>
-      <c r="L85" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="M85" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="N85" s="16" t="str">
+      <c r="L85" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="M85" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="N85" s="62" t="str">
         <f t="shared" ref="N85" si="231">W85</f>
         <v>E2</v>
       </c>
-      <c r="O85" s="19" t="str">
+      <c r="O85" s="65" t="str">
         <f t="shared" ref="O85" si="232">"FF01"&amp;J85&amp;""&amp;K85&amp;L85&amp;M85&amp;N85</f>
         <v>FF01A1400000E2</v>
       </c>
-      <c r="P85" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q85" s="21">
+      <c r="P85" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q85" s="67">
         <f t="shared" ref="Q85" si="233">HEX2DEC(I85)</f>
         <v>1</v>
       </c>
-      <c r="R85" s="21">
+      <c r="R85" s="67">
         <f t="shared" ref="R85" si="234">HEX2DEC(J85)</f>
         <v>161</v>
       </c>
-      <c r="S85" s="21">
+      <c r="S85" s="67">
         <f t="shared" ref="S85" si="235">HEX2DEC(K85)</f>
         <v>64</v>
       </c>
-      <c r="T85" s="21">
+      <c r="T85" s="67">
         <f t="shared" ref="T85" si="236">HEX2DEC(L85)</f>
         <v>0</v>
       </c>
-      <c r="U85" s="21">
+      <c r="U85" s="67">
         <f t="shared" ref="U85" si="237">HEX2DEC(M85)</f>
         <v>0</v>
       </c>
-      <c r="V85" s="21">
+      <c r="V85" s="67">
         <f t="shared" ref="V85" si="238">SUM(Q85:U85)</f>
         <v>226</v>
       </c>
-      <c r="W85" s="21" t="str">
+      <c r="W85" s="68" t="str">
         <f t="shared" si="230"/>
         <v>E2</v>
       </c>
     </row>
     <row r="86" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="16" t="s">
+      <c r="B86" s="81" t="s">
         <v>150</v>
       </c>
-      <c r="C86" s="16"/>
+      <c r="C86" s="73"/>
       <c r="D86" s="16"/>
       <c r="E86" s="16"/>
       <c r="F86" s="16"/>
@@ -7521,16 +7823,16 @@
         <f t="shared" ref="V86" si="246">SUM(Q86:U86)</f>
         <v>226</v>
       </c>
-      <c r="W86" s="21" t="str">
+      <c r="W86" s="61" t="str">
         <f t="shared" si="230"/>
         <v>E2</v>
       </c>
     </row>
     <row r="87" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="81" t="s">
         <v>151</v>
       </c>
-      <c r="C87" s="16"/>
+      <c r="C87" s="73"/>
       <c r="D87" s="16"/>
       <c r="E87" s="16"/>
       <c r="F87" s="16"/>
@@ -7586,16 +7888,16 @@
         <f t="shared" ref="V87:V91" si="254">SUM(Q87:U87)</f>
         <v>227</v>
       </c>
-      <c r="W87" s="21" t="str">
+      <c r="W87" s="61" t="str">
         <f t="shared" si="230"/>
         <v>E3</v>
       </c>
     </row>
     <row r="88" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="16" t="s">
+      <c r="B88" s="81" t="s">
         <v>152</v>
       </c>
-      <c r="C88" s="16"/>
+      <c r="C88" s="73"/>
       <c r="D88" s="16"/>
       <c r="E88" s="16"/>
       <c r="F88" s="16"/>
@@ -7651,16 +7953,16 @@
         <f t="shared" si="254"/>
         <v>228</v>
       </c>
-      <c r="W88" s="21" t="str">
+      <c r="W88" s="61" t="str">
         <f t="shared" si="230"/>
         <v>E4</v>
       </c>
     </row>
     <row r="89" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="C89" s="16"/>
+      <c r="C89" s="73"/>
       <c r="D89" s="16"/>
       <c r="E89" s="16"/>
       <c r="F89" s="16"/>
@@ -7716,16 +8018,16 @@
         <f t="shared" si="254"/>
         <v>229</v>
       </c>
-      <c r="W89" s="21" t="str">
+      <c r="W89" s="61" t="str">
         <f t="shared" si="230"/>
         <v>E5</v>
       </c>
     </row>
     <row r="90" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="16" t="s">
+      <c r="B90" s="81" t="s">
         <v>154</v>
       </c>
-      <c r="C90" s="16"/>
+      <c r="C90" s="73"/>
       <c r="D90" s="16"/>
       <c r="E90" s="16"/>
       <c r="F90" s="16"/>
@@ -7781,74 +8083,89 @@
         <f t="shared" si="254"/>
         <v>229</v>
       </c>
-      <c r="W90" s="21" t="str">
+      <c r="W90" s="61" t="str">
         <f t="shared" si="230"/>
         <v>E5</v>
       </c>
     </row>
-    <row r="91" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="16" t="s">
+    <row r="91" spans="2:23" s="2" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="78" t="s">
         <v>155</v>
       </c>
-      <c r="C91" s="16"/>
-      <c r="D91" s="16"/>
-      <c r="E91" s="16"/>
-      <c r="F91" s="16"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="16"/>
-      <c r="I91" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="J91" s="16" t="s">
+      <c r="C91" s="72"/>
+      <c r="D91" s="32"/>
+      <c r="E91" s="32"/>
+      <c r="F91" s="32"/>
+      <c r="G91" s="33"/>
+      <c r="H91" s="32"/>
+      <c r="I91" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="J91" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="K91" s="16">
+      <c r="K91" s="32">
         <v>43</v>
       </c>
-      <c r="L91" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="M91" s="18" t="s">
+      <c r="L91" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="M91" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="N91" s="16" t="str">
+      <c r="N91" s="32" t="str">
         <f t="shared" si="247"/>
         <v>98</v>
       </c>
-      <c r="O91" s="19" t="str">
+      <c r="O91" s="35" t="str">
         <f t="shared" si="248"/>
         <v>FF01A04300B498</v>
       </c>
-      <c r="P91" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q91" s="21">
+      <c r="P91" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q91" s="37">
         <f t="shared" si="249"/>
         <v>1</v>
       </c>
-      <c r="R91" s="21">
+      <c r="R91" s="37">
         <f t="shared" si="250"/>
         <v>160</v>
       </c>
-      <c r="S91" s="21">
+      <c r="S91" s="37">
         <f t="shared" si="251"/>
         <v>67</v>
       </c>
-      <c r="T91" s="21">
+      <c r="T91" s="37">
         <f t="shared" si="252"/>
         <v>0</v>
       </c>
-      <c r="U91" s="21">
+      <c r="U91" s="37">
         <f t="shared" si="253"/>
         <v>180</v>
       </c>
-      <c r="V91" s="21">
+      <c r="V91" s="37">
         <f t="shared" si="254"/>
         <v>408</v>
       </c>
-      <c r="W91" s="21" t="str">
+      <c r="W91" s="38" t="str">
         <f t="shared" si="230"/>
         <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="2:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="83" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="93" spans="2:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="83" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="2:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="83" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -11798,7 +12115,7 @@
         <v>9</v>
       </c>
       <c r="Q61" s="15">
-        <f t="shared" ref="Q61:U69" si="19">HEX2DEC(I61)</f>
+        <f t="shared" ref="Q61:U62" si="19">HEX2DEC(I61)</f>
         <v>1</v>
       </c>
       <c r="R61" s="15">
@@ -12208,7 +12525,7 @@
         <v>1</v>
       </c>
       <c r="V67" s="15">
-        <f t="shared" ref="V67:V131" si="23">SUM(Q67:U67)</f>
+        <f t="shared" ref="V67:V102" si="23">SUM(Q67:U67)</f>
         <v>196</v>
       </c>
       <c r="W67" s="30" t="str">

</xml_diff>

<commit_message>
2024.10.17 1) (2024.09.24): PTZ func for FT 2) (2024.09.24): Add RTSP for FT 3) (2024.09.24): Add Model for FT 4) (2024.09.25) Find selected model 5) (2024.09.25): add a PTZ 8 Direction UI(move toggle sw and set button) 6) (2024.09.26) Add diagonal direction Button 7) (2024.09.30): Create preset file 8) (2024.10.02): Initialize a Preset UI 9) (2024.10.06): Save/Call a Preset 10) (2024.10.10): Sava/Call a Tour 11) (2024.10.14): Applied Http Digest
</commit_message>
<xml_diff>
--- a/Command/Command.xlsx
+++ b/Command/Command.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Project\Python\TestTool\Command\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE693A4-0709-433C-ADA9-4CA736E0DEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294F8A7B-2CB9-4CD0-85BF-21FDA1B00232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{79FED000-970D-0E48-B65E-FB5160DD82FF}"/>
+    <workbookView xWindow="33480" yWindow="2325" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{79FED000-970D-0E48-B65E-FB5160DD82FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Uncooled" sheetId="1" r:id="rId1"/>
     <sheet name="NYX Series" sheetId="5" r:id="rId2"/>
     <sheet name="DRS" sheetId="7" r:id="rId3"/>
-    <sheet name="Uncooled Data Sheet" sheetId="2" r:id="rId4"/>
-    <sheet name="Cooled Data Sheet" sheetId="6" r:id="rId5"/>
-    <sheet name="CMD RAW" sheetId="3" r:id="rId6"/>
+    <sheet name="FineTree" sheetId="8" r:id="rId4"/>
+    <sheet name="Uncooled Data Sheet" sheetId="2" r:id="rId5"/>
+    <sheet name="Cooled Data Sheet" sheetId="6" r:id="rId6"/>
+    <sheet name="CMD RAW" sheetId="3" r:id="rId7"/>
+    <sheet name="FineTreeRAW" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'NYX Series'!$B$2:$N$259</definedName>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3417" uniqueCount="1135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4002" uniqueCount="1266">
   <si>
     <r>
       <rPr>
@@ -4389,6 +4391,528 @@
   </si>
   <si>
     <t>Gamma Filter 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rev.2024.09.26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>move</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>focus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BaseURL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pspd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pan Spd 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pan Spd 63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tspd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tilt Spd 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tilt Spd 63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zspd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max 63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom Spd 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom Spd 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zoom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom Tele Step 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zoom Wide Step 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>near</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>far</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus Near</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus Far</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus Far Step 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus Near Step 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PTZ Stop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>preset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Preset 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pre+71 Wiper Run</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pre+77 Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pre+76 Night</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pre+87 Reverse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pre+88 Normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Preset 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus Auto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus Manual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group,app,flip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic,set,enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic,set,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>af,set,auto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>af,set,manual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group,app,mirror</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/cgi-bin/ptz/control.php</t>
+  </si>
+  <si>
+    <t>/setup/video/image.php</t>
+  </si>
+  <si>
+    <t>NTSC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,video_mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,NTSC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,PAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/setup/video/source.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,1920x1080_30fps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,1920x1080_60fps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source 1920x1080 30fps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source 1920x1080 60fps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,video_src</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/setup/video/stream.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,H265MP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H.265 Main Profile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H.264 Main Profile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,H264MP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,video_enc#_codec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MJPEG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,MJPEG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,video_enc#_fps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 fps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30 fps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60 fps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus PushAF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>af,set,pushaf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group,app,focus_mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group,app,focus_speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>af,set,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>af,set,8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>focus spd 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>focus spd 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group,app,dnn_mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dnn,set,auto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D/N Auto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D/N Day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D/N Night</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D/N Ext</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dnn,set,day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dnn,set,night</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dnn,set,ext</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WDR On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WDR Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defog On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defog Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group,app,wdr_mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wdr,set,on</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wdr,set,off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group,app,defog_mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blc,set,off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blc,set,on</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group,app,blc_mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BLC On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BLC Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HLC On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HLC Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group,app,hlc_mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/setup/video/digital_zoom.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,dz_enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D-Zoom Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D-Zoom On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set,800</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,dz_level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Restart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/setup/system/restart.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Except IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Include IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/setup/system/reset.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/setup/system/default.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,video_enc1_fps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,video_enc1_codec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/cgi-bin/ptz/control.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pushaf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,restart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app,default</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5002,7 +5526,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5275,6 +5799,9 @@
     </xf>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -16637,7 +17164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E92AE5-296A-4A53-A69F-D6F31FDFEA61}">
   <dimension ref="B1:T156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
@@ -26581,6 +27108,1300 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94EB275-FA34-45A8-B46C-8DC3CCB3E735}">
+  <dimension ref="B1:H58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
+  <cols>
+    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" style="80" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8">
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="H1" s="80" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" s="2" customFormat="1">
+      <c r="B2" s="86" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="86" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E2" s="86" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F2" s="86" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G2" s="86" t="s">
+        <v>312</v>
+      </c>
+      <c r="H2" s="86" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="88" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C3" s="88" t="str">
+        <f t="shared" ref="C3:C12" si="0">IF(G3="get", D3, D3&amp;"="&amp;E3)</f>
+        <v>app,video_mode=set,NTSC</v>
+      </c>
+      <c r="D3" s="88" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E3" s="88" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F3" s="88" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G3" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H3" s="88"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="88" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C4" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_mode=set,PAL</v>
+      </c>
+      <c r="D4" s="88" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E4" s="88" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F4" s="88" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G4" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H4" s="88"/>
+    </row>
+    <row r="5" spans="2:8" ht="27">
+      <c r="B5" s="88" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C5" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_src=set,1920x1080_30fps</v>
+      </c>
+      <c r="D5" s="88" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E5" s="88" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F5" s="88" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G5" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H5" s="88"/>
+    </row>
+    <row r="6" spans="2:8" ht="27">
+      <c r="B6" s="88" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C6" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_src=set,1920x1080_60fps</v>
+      </c>
+      <c r="D6" s="88" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E6" s="88" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F6" s="88" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G6" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H6" s="88"/>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="88" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C7" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_enc1_codec=set,H265MP</v>
+      </c>
+      <c r="D7" s="88" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E7" s="88" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F7" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G7" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H7" s="88"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="88" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C8" s="88" t="str">
+        <f t="shared" ref="C8:C9" si="1">IF(G8="get", D8, D8&amp;"="&amp;E8)</f>
+        <v>app,video_enc1_codec=set,H264MP</v>
+      </c>
+      <c r="D8" s="88" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E8" s="88" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F8" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G8" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H8" s="88"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="88" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C9" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>app,video_enc1_codec=set,MJPEG</v>
+      </c>
+      <c r="D9" s="88" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E9" s="88" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F9" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G9" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H9" s="88"/>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="88" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C10" s="88" t="str">
+        <f t="shared" ref="C10:C11" si="2">IF(G10="get", D10, D10&amp;"="&amp;E10)</f>
+        <v>app,video_enc1_fps=set,1</v>
+      </c>
+      <c r="D10" s="88" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E10" s="88" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F10" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G10" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H10" s="88"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="88" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C11" s="88" t="str">
+        <f t="shared" si="2"/>
+        <v>app,video_enc1_fps=set,30</v>
+      </c>
+      <c r="D11" s="88" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E11" s="88" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F11" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G11" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H11" s="88"/>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="88" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C12" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_enc1_fps=set,60</v>
+      </c>
+      <c r="D12" s="88" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E12" s="88" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F12" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G12" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H12" s="88"/>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="88" t="str">
+        <f>IF(G13="get", D13, D13&amp;"="&amp;E13)</f>
+        <v>group,app,flip=basic,set,enable</v>
+      </c>
+      <c r="D13" s="88" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E13" s="88" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F13" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G13" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H13" s="88"/>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="88" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="88" t="str">
+        <f t="shared" ref="C14:C16" si="3">IF(G14="get", D14, D14&amp;"="&amp;E14)</f>
+        <v>group,app,flip=basic,set,1</v>
+      </c>
+      <c r="D14" s="88" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E14" s="88" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F14" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G14" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H14" s="88"/>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="88" t="str">
+        <f t="shared" si="3"/>
+        <v>group,app,mirror=basic,set,enable</v>
+      </c>
+      <c r="D15" s="88" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E15" s="88" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F15" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G15" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H15" s="88"/>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="88" t="str">
+        <f t="shared" si="3"/>
+        <v>group,app,mirror=basic,set,1</v>
+      </c>
+      <c r="D16" s="88" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E16" s="88" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F16" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G16" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H16" s="88"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="88" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C17" s="88" t="str">
+        <f t="shared" ref="C17" si="4">IF(G17="get", D17, D17&amp;"="&amp;E17)</f>
+        <v>group,app,focus_mode=af,set,auto</v>
+      </c>
+      <c r="D17" s="88" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E17" s="88" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F17" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G17" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H17" s="88"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="88" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C18" s="88" t="str">
+        <f t="shared" ref="C18:C27" si="5">IF(G18="get", D18, D18&amp;"="&amp;E18)</f>
+        <v>group,app,focus_mode=af,set,manual</v>
+      </c>
+      <c r="D18" s="88" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E18" s="88" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F18" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G18" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H18" s="88"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="88" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C19" s="88" t="str">
+        <f t="shared" ref="C19:C23" si="6">IF(G19="get", D19, D19&amp;"="&amp;E19)</f>
+        <v>focus=pushaf</v>
+      </c>
+      <c r="D19" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E19" s="88" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F19" s="93" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G19" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H19" s="88"/>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="88" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C20" s="88" t="str">
+        <f t="shared" si="6"/>
+        <v>group,app,focus_speed=af,set,1</v>
+      </c>
+      <c r="D20" s="88" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E20" s="88" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F20" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G20" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H20" s="88"/>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="88" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C21" s="88" t="str">
+        <f t="shared" si="6"/>
+        <v>group,app,focus_speed=af,set,8</v>
+      </c>
+      <c r="D21" s="88" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E21" s="88" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F21" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G21" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H21" s="88"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="88" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C22" s="88" t="str">
+        <f t="shared" si="6"/>
+        <v>group,app,dnn_mode=dnn,set,auto</v>
+      </c>
+      <c r="D22" s="88" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E22" s="88" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F22" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G22" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H22" s="88"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="88" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C23" s="88" t="str">
+        <f t="shared" si="6"/>
+        <v>group,app,dnn_mode=dnn,set,day</v>
+      </c>
+      <c r="D23" s="88" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E23" s="88" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F23" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G23" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H23" s="88"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="88" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C24" s="88" t="str">
+        <f t="shared" si="5"/>
+        <v>group,app,dnn_mode=dnn,set,night</v>
+      </c>
+      <c r="D24" s="88" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E24" s="88" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F24" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G24" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H24" s="88"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="88" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C25" s="88" t="str">
+        <f t="shared" si="5"/>
+        <v>group,app,dnn_mode=dnn,set,ext</v>
+      </c>
+      <c r="D25" s="88" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E25" s="88" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F25" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G25" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H25" s="88"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="88" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C26" s="88" t="str">
+        <f t="shared" si="5"/>
+        <v>group,app,wdr_mode=wdr,set,on</v>
+      </c>
+      <c r="D26" s="88" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E26" s="88" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F26" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G26" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H26" s="88"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="88" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C27" s="88" t="str">
+        <f t="shared" si="5"/>
+        <v>group,app,wdr_mode=wdr,set,off</v>
+      </c>
+      <c r="D27" s="88" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E27" s="88" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F27" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G27" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H27" s="88"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="88" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C28" s="88" t="str">
+        <f t="shared" ref="C28:C37" si="7">IF(G28="get", D28, D28&amp;"="&amp;E28)</f>
+        <v>group,app,defog_mode=wdr,set,on</v>
+      </c>
+      <c r="D28" s="88" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E28" s="88" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F28" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G28" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H28" s="88"/>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="88" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C29" s="88" t="str">
+        <f t="shared" si="7"/>
+        <v>group,app,defog_mode=wdr,set,off</v>
+      </c>
+      <c r="D29" s="88" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E29" s="88" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F29" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G29" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H29" s="88"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="88" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C30" s="88" t="str">
+        <f t="shared" si="7"/>
+        <v>group,app,blc_mode=blc,set,on</v>
+      </c>
+      <c r="D30" s="88" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E30" s="88" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F30" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G30" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H30" s="88"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="88" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C31" s="88" t="str">
+        <f t="shared" si="7"/>
+        <v>group,app,blc_mode=blc,set,off</v>
+      </c>
+      <c r="D31" s="88" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E31" s="88" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F31" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G31" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H31" s="88"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="88" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C32" s="88" t="str">
+        <f t="shared" si="7"/>
+        <v>group,app,hlc_mode=blc,set,on</v>
+      </c>
+      <c r="D32" s="88" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E32" s="88" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F32" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G32" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H32" s="88"/>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="88" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C33" s="88" t="str">
+        <f t="shared" si="7"/>
+        <v>group,app,hlc_mode=blc,set,off</v>
+      </c>
+      <c r="D33" s="88" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E33" s="88" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F33" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G33" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H33" s="88"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="88" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C34" s="88" t="str">
+        <f t="shared" si="7"/>
+        <v>app,dz_enable=set,0</v>
+      </c>
+      <c r="D34" s="88" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E34" s="88" t="s">
+        <v>1242</v>
+      </c>
+      <c r="F34" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G34" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H34" s="88"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="88" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C35" s="88" t="str">
+        <f t="shared" si="7"/>
+        <v>app,dz_enable=set,1</v>
+      </c>
+      <c r="D35" s="88" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E35" s="88" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F35" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G35" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H35" s="88"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="88" t="s">
+        <v>972</v>
+      </c>
+      <c r="C36" s="88" t="str">
+        <f t="shared" si="7"/>
+        <v>app,dz_level=set,100</v>
+      </c>
+      <c r="D36" s="88" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E36" s="88" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F36" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G36" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H36" s="88"/>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="88" t="s">
+        <v>974</v>
+      </c>
+      <c r="C37" s="88" t="str">
+        <f t="shared" si="7"/>
+        <v>app,dz_level=set,200</v>
+      </c>
+      <c r="D37" s="88" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E37" s="88" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F37" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G37" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H37" s="88"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="88" t="s">
+        <v>975</v>
+      </c>
+      <c r="C38" s="88" t="str">
+        <f t="shared" ref="C38:C41" si="8">IF(G38="get", D38, D38&amp;"="&amp;E38)</f>
+        <v>app,dz_level=set,400</v>
+      </c>
+      <c r="D38" s="88" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E38" s="88" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F38" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G38" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H38" s="88"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="88" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C39" s="88" t="str">
+        <f t="shared" si="8"/>
+        <v>app,dz_level=set,800</v>
+      </c>
+      <c r="D39" s="88" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E39" s="88" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F39" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G39" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H39" s="88"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="88" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C40" s="88" t="str">
+        <f t="shared" si="8"/>
+        <v>app,restart=set,1</v>
+      </c>
+      <c r="D40" s="88" t="s">
+        <v>1263</v>
+      </c>
+      <c r="E40" s="88" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F40" s="88" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G40" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H40" s="88"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="88" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C41" s="88" t="str">
+        <f t="shared" si="8"/>
+        <v>app,reset=set,1</v>
+      </c>
+      <c r="D41" s="88" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E41" s="88" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F41" s="88" t="s">
+        <v>1257</v>
+      </c>
+      <c r="G41" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H41" s="88" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="88" t="s">
+        <v>578</v>
+      </c>
+      <c r="C42" s="88" t="str">
+        <f t="shared" ref="C42:C58" si="9">IF(G42="get", D42, D42&amp;"="&amp;E42)</f>
+        <v>app,default=set,1</v>
+      </c>
+      <c r="D42" s="88" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E42" s="88" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F42" s="88" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G42" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H42" s="88" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="88" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C43" s="88" t="str">
+        <f t="shared" ref="C43:C51" si="10">IF(G43="get", D43, D43&amp;"="&amp;E43)</f>
+        <v>pspd=1</v>
+      </c>
+      <c r="D43" s="88" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E43" s="88">
+        <v>1</v>
+      </c>
+      <c r="F43" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G43" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H43" s="88" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="88" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C44" s="88" t="str">
+        <f t="shared" si="10"/>
+        <v>pspd=63</v>
+      </c>
+      <c r="D44" s="88" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E44" s="88">
+        <v>63</v>
+      </c>
+      <c r="F44" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G44" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H44" s="88"/>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="88" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C45" s="88" t="str">
+        <f t="shared" si="10"/>
+        <v>tspd=1</v>
+      </c>
+      <c r="D45" s="88" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E45" s="88">
+        <v>1</v>
+      </c>
+      <c r="F45" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G45" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H45" s="88" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="88" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C46" s="88" t="str">
+        <f t="shared" si="10"/>
+        <v>tspd=63</v>
+      </c>
+      <c r="D46" s="88" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E46" s="88">
+        <v>63</v>
+      </c>
+      <c r="F46" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G46" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H46" s="88"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="88" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C47" s="88" t="str">
+        <f t="shared" si="10"/>
+        <v>zspd=1</v>
+      </c>
+      <c r="D47" s="88" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E47" s="88">
+        <v>1</v>
+      </c>
+      <c r="F47" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G47" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H47" s="88" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="88" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C48" s="88" t="str">
+        <f t="shared" si="10"/>
+        <v>zspd=8</v>
+      </c>
+      <c r="D48" s="88" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E48" s="88">
+        <v>8</v>
+      </c>
+      <c r="F48" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G48" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H48" s="88"/>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="88" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C49" s="88" t="str">
+        <f t="shared" si="10"/>
+        <v>zoom=1</v>
+      </c>
+      <c r="D49" s="88" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E49" s="88">
+        <v>1</v>
+      </c>
+      <c r="F49" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G49" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H49" s="88"/>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="88" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C50" s="88" t="str">
+        <f t="shared" si="10"/>
+        <v>zoom=1</v>
+      </c>
+      <c r="D50" s="88" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E50" s="88">
+        <v>1</v>
+      </c>
+      <c r="F50" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G50" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H50" s="88"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="88" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C51" s="88" t="str">
+        <f t="shared" si="10"/>
+        <v>zoom=stop</v>
+      </c>
+      <c r="D51" s="88" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E51" s="88" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F51" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G51" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H51" s="88"/>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="88" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C52" s="88" t="str">
+        <f t="shared" ref="C52:C57" si="11">IF(G52="get", D52, D52&amp;"="&amp;E52)</f>
+        <v>focus=near</v>
+      </c>
+      <c r="D52" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E52" s="88" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F52" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G52" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H52" s="88"/>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="88" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C53" s="88" t="str">
+        <f t="shared" si="11"/>
+        <v>focus=far</v>
+      </c>
+      <c r="D53" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E53" s="88" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F53" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G53" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H53" s="88"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="88" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C54" s="88" t="str">
+        <f t="shared" si="11"/>
+        <v>focus=1</v>
+      </c>
+      <c r="D54" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E54" s="88">
+        <v>1</v>
+      </c>
+      <c r="F54" s="88" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G54" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H54" s="88"/>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="88" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C55" s="88" t="str">
+        <f t="shared" si="11"/>
+        <v>focus=1</v>
+      </c>
+      <c r="D55" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E55" s="88">
+        <v>1</v>
+      </c>
+      <c r="F55" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G55" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H55" s="88"/>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="88" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C56" s="88" t="str">
+        <f t="shared" si="11"/>
+        <v>focus=stop</v>
+      </c>
+      <c r="D56" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E56" s="88" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F56" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G56" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H56" s="88"/>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="88" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C57" s="88" t="str">
+        <f t="shared" si="11"/>
+        <v>move=stop</v>
+      </c>
+      <c r="D57" s="88" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E57" s="88" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F57" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G57" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H57" s="88"/>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="88"/>
+      <c r="C58" s="88" t="str">
+        <f t="shared" si="9"/>
+        <v>=FALSE</v>
+      </c>
+      <c r="D58" s="88"/>
+      <c r="E58" s="88" t="b">
+        <f t="shared" ref="E58" si="12">IF(G58="get", "")</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="88"/>
+      <c r="G58" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H58" s="88"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4216FE-61C8-B941-B13D-072D42E23E52}">
   <dimension ref="B1:H1"/>
   <sheetViews>
@@ -26608,7 +28429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FA9FE0-2B56-4EB8-B96C-F19E41E24CE4}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -26624,7 +28445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0BD130-7E94-4798-80EB-E2350D9BAC78}">
   <dimension ref="B1:X102"/>
   <sheetViews>
@@ -33538,4 +35359,1468 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E8CE7D-D20F-41DE-9075-E508ED12C670}">
+  <dimension ref="B1:H66"/>
+  <sheetViews>
+    <sheetView topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25"/>
+  <cols>
+    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" style="80" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8">
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="H1" s="80" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" s="2" customFormat="1">
+      <c r="B2" s="86" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="86" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E2" s="86" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F2" s="86" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G2" s="86" t="s">
+        <v>312</v>
+      </c>
+      <c r="H2" s="86" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="88" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C3" s="88" t="str">
+        <f t="shared" ref="C3:C19" si="0">IF(G3="get", D3, D3&amp;"="&amp;E3)</f>
+        <v>preset=1</v>
+      </c>
+      <c r="D3" s="88" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E3" s="88">
+        <v>1</v>
+      </c>
+      <c r="F3" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G3" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H3" s="88"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="88" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C4" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>preset=8</v>
+      </c>
+      <c r="D4" s="88" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E4" s="88">
+        <v>8</v>
+      </c>
+      <c r="F4" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G4" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H4" s="88"/>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="88" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C5" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>preset=71</v>
+      </c>
+      <c r="D5" s="88" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E5" s="88">
+        <v>71</v>
+      </c>
+      <c r="F5" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G5" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H5" s="88"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="88" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C6" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>preset=76</v>
+      </c>
+      <c r="D6" s="88" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E6" s="88">
+        <v>76</v>
+      </c>
+      <c r="F6" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G6" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H6" s="88"/>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="88" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C7" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>preset=77</v>
+      </c>
+      <c r="D7" s="88" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E7" s="88">
+        <v>77</v>
+      </c>
+      <c r="F7" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G7" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H7" s="88"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="88" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C8" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>preset=87</v>
+      </c>
+      <c r="D8" s="88" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E8" s="88">
+        <v>87</v>
+      </c>
+      <c r="F8" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G8" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H8" s="88"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="88" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C9" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>preset=88</v>
+      </c>
+      <c r="D9" s="88" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E9" s="88">
+        <v>88</v>
+      </c>
+      <c r="F9" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G9" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H9" s="88"/>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="88" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C10" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_mode=set,NTSC</v>
+      </c>
+      <c r="D10" s="88" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E10" s="88" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F10" s="88" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G10" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H10" s="88"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="88" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C11" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_mode=set,PAL</v>
+      </c>
+      <c r="D11" s="88" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E11" s="88" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F11" s="88" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G11" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H11" s="88"/>
+    </row>
+    <row r="12" spans="2:8" ht="27">
+      <c r="B12" s="88" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C12" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_src=set,1920x1080_30fps</v>
+      </c>
+      <c r="D12" s="88" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E12" s="88" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F12" s="88" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G12" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H12" s="88"/>
+    </row>
+    <row r="13" spans="2:8" ht="27">
+      <c r="B13" s="88" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C13" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_src=set,1920x1080_60fps</v>
+      </c>
+      <c r="D13" s="88" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E13" s="88" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F13" s="88" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G13" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H13" s="88"/>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="88" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C14" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_enc#_codec=set,H265MP</v>
+      </c>
+      <c r="D14" s="88" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E14" s="88" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F14" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G14" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H14" s="88"/>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="88" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C15" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_enc#_codec=set,H264MP</v>
+      </c>
+      <c r="D15" s="88" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E15" s="88" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F15" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G15" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H15" s="88"/>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="88" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C16" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_enc#_codec=set,MJPEG</v>
+      </c>
+      <c r="D16" s="88" t="s">
+        <v>1198</v>
+      </c>
+      <c r="E16" s="88" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F16" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G16" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H16" s="88"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="88" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C17" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_enc#_fps=set,1</v>
+      </c>
+      <c r="D17" s="88" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E17" s="88" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F17" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G17" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H17" s="88"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="88" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C18" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_enc#_fps=set,30</v>
+      </c>
+      <c r="D18" s="88" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E18" s="88" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F18" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G18" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H18" s="88"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="88" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C19" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>app,video_enc#_fps=set,60</v>
+      </c>
+      <c r="D19" s="88" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E19" s="88" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F19" s="88" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G19" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H19" s="88"/>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="88" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="88" t="str">
+        <f>IF(G20="get", D20, D20&amp;"="&amp;E20)</f>
+        <v>group,app,flip=basic,set,enable</v>
+      </c>
+      <c r="D20" s="88" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E20" s="88" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F20" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G20" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H20" s="88"/>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="88" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="88" t="str">
+        <f t="shared" ref="C21:C66" si="1">IF(G21="get", D21, D21&amp;"="&amp;E21)</f>
+        <v>group,app,flip=basic,set,1</v>
+      </c>
+      <c r="D21" s="88" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E21" s="88" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F21" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G21" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H21" s="88"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,mirror=basic,set,enable</v>
+      </c>
+      <c r="D22" s="88" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E22" s="88" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F22" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G22" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H22" s="88"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,mirror=basic,set,1</v>
+      </c>
+      <c r="D23" s="88" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E23" s="88" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F23" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G23" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H23" s="88"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="88" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C24" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,focus_mode=af,set,auto</v>
+      </c>
+      <c r="D24" s="88" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E24" s="88" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F24" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G24" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H24" s="88"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="88" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C25" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,focus_mode=af,set,manual</v>
+      </c>
+      <c r="D25" s="88" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E25" s="88" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F25" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G25" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H25" s="88"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="88" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C26" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,focus_mode=af,set,pushaf</v>
+      </c>
+      <c r="D26" s="88" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E26" s="88" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F26" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G26" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H26" s="88"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="88" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C27" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,focus_speed=af,set,1</v>
+      </c>
+      <c r="D27" s="88" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E27" s="88" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F27" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G27" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H27" s="88"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="88" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C28" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,focus_speed=af,set,8</v>
+      </c>
+      <c r="D28" s="88" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E28" s="88" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F28" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G28" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H28" s="88"/>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="88" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C29" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,dnn_mode=dnn,set,auto</v>
+      </c>
+      <c r="D29" s="88" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E29" s="88" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F29" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G29" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H29" s="88"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="88" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C30" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,dnn_mode=dnn,set,day</v>
+      </c>
+      <c r="D30" s="88" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E30" s="88" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F30" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G30" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H30" s="88"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="88" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C31" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,dnn_mode=dnn,set,night</v>
+      </c>
+      <c r="D31" s="88" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E31" s="88" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F31" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G31" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H31" s="88"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="88" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C32" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,dnn_mode=dnn,set,ext</v>
+      </c>
+      <c r="D32" s="88" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E32" s="88" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F32" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G32" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H32" s="88"/>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="88" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C33" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,wdr_mode=wdr,set,on</v>
+      </c>
+      <c r="D33" s="88" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E33" s="88" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F33" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G33" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H33" s="88"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="88" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C34" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,wdr_mode=wdr,set,off</v>
+      </c>
+      <c r="D34" s="88" t="s">
+        <v>1229</v>
+      </c>
+      <c r="E34" s="88" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F34" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G34" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H34" s="88"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="88" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C35" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,defog_mode=wdr,set,on</v>
+      </c>
+      <c r="D35" s="88" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E35" s="88" t="s">
+        <v>1230</v>
+      </c>
+      <c r="F35" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G35" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H35" s="88"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="88" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C36" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,defog_mode=wdr,set,off</v>
+      </c>
+      <c r="D36" s="88" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E36" s="88" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F36" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G36" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H36" s="88"/>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="88" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C37" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,blc_mode=blc,set,on</v>
+      </c>
+      <c r="D37" s="88" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E37" s="88" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F37" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G37" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H37" s="88"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="88" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C38" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,blc_mode=blc,set,off</v>
+      </c>
+      <c r="D38" s="88" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E38" s="88" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F38" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G38" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H38" s="88"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="88" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C39" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,hlc_mode=blc,set,on</v>
+      </c>
+      <c r="D39" s="88" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E39" s="88" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F39" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G39" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H39" s="88"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="88" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C40" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>group,app,hlc_mode=blc,set,off</v>
+      </c>
+      <c r="D40" s="88" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E40" s="88" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F40" s="88" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G40" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H40" s="88"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="88" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C41" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>app,dz_enable=set,0</v>
+      </c>
+      <c r="D41" s="88" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E41" s="88" t="s">
+        <v>1242</v>
+      </c>
+      <c r="F41" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G41" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H41" s="88"/>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="88" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C42" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>app,dz_enable=set,1</v>
+      </c>
+      <c r="D42" s="88" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E42" s="88" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F42" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G42" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H42" s="88"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="88" t="s">
+        <v>972</v>
+      </c>
+      <c r="C43" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>app,dz_level=set,100</v>
+      </c>
+      <c r="D43" s="88" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E43" s="88" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F43" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G43" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H43" s="88"/>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="88" t="s">
+        <v>974</v>
+      </c>
+      <c r="C44" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>app,dz_level=set,200</v>
+      </c>
+      <c r="D44" s="88" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E44" s="88" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F44" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G44" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H44" s="88"/>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="88" t="s">
+        <v>975</v>
+      </c>
+      <c r="C45" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>app,dz_level=set,400</v>
+      </c>
+      <c r="D45" s="88" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E45" s="88" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F45" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G45" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H45" s="88"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="88" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C46" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>app,dz_level=set,800</v>
+      </c>
+      <c r="D46" s="88" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E46" s="88" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F46" s="88" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G46" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H46" s="88"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="88" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C47" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>app=set</v>
+      </c>
+      <c r="D47" s="88" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E47" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F47" s="88" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G47" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H47" s="88"/>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="88" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C48" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>app=set</v>
+      </c>
+      <c r="D48" s="88" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E48" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F48" s="88" t="s">
+        <v>1257</v>
+      </c>
+      <c r="G48" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H48" s="88" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="88" t="s">
+        <v>578</v>
+      </c>
+      <c r="C49" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>=FALSE</v>
+      </c>
+      <c r="D49" s="88"/>
+      <c r="E49" s="88" t="b">
+        <f t="shared" ref="E49:E66" si="2">IF(G49="get", "")</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="88" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G49" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H49" s="88" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="88" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C50" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>pspd=1</v>
+      </c>
+      <c r="D50" s="88" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E50" s="88">
+        <v>1</v>
+      </c>
+      <c r="F50" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G50" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H50" s="88" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="88" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C51" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>pspd=63</v>
+      </c>
+      <c r="D51" s="88" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E51" s="88">
+        <v>63</v>
+      </c>
+      <c r="F51" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G51" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H51" s="88"/>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="88" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C52" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>tspd=1</v>
+      </c>
+      <c r="D52" s="88" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E52" s="88">
+        <v>1</v>
+      </c>
+      <c r="F52" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G52" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H52" s="88" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="88" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C53" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>tspd=63</v>
+      </c>
+      <c r="D53" s="88" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E53" s="88">
+        <v>63</v>
+      </c>
+      <c r="F53" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G53" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H53" s="88"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="88" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C54" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>zspd=1</v>
+      </c>
+      <c r="D54" s="88" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E54" s="88">
+        <v>1</v>
+      </c>
+      <c r="F54" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G54" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H54" s="88" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="88" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C55" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>zspd=8</v>
+      </c>
+      <c r="D55" s="88" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E55" s="88">
+        <v>8</v>
+      </c>
+      <c r="F55" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G55" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H55" s="88"/>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="88" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C56" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>zoom=1</v>
+      </c>
+      <c r="D56" s="88" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E56" s="88">
+        <v>1</v>
+      </c>
+      <c r="F56" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G56" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H56" s="88"/>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="88" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C57" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>zoom=1</v>
+      </c>
+      <c r="D57" s="88" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E57" s="88">
+        <v>1</v>
+      </c>
+      <c r="F57" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G57" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H57" s="88"/>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="88" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C58" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>zoom=stop</v>
+      </c>
+      <c r="D58" s="88" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E58" s="88" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F58" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G58" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H58" s="88"/>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" s="88" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C59" s="88" t="str">
+        <f t="shared" ref="C59:C64" si="3">IF(G59="get", D59, D59&amp;"="&amp;E59)</f>
+        <v>focus=near</v>
+      </c>
+      <c r="D59" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E59" s="88" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F59" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G59" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H59" s="88"/>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60" s="88" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C60" s="88" t="str">
+        <f t="shared" si="3"/>
+        <v>focus=far</v>
+      </c>
+      <c r="D60" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E60" s="88" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F60" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G60" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H60" s="88"/>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" s="88" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C61" s="88" t="str">
+        <f t="shared" si="3"/>
+        <v>focus=1</v>
+      </c>
+      <c r="D61" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E61" s="88">
+        <v>1</v>
+      </c>
+      <c r="F61" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G61" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H61" s="88"/>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62" s="88" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C62" s="88" t="str">
+        <f t="shared" si="3"/>
+        <v>focus=1</v>
+      </c>
+      <c r="D62" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E62" s="88">
+        <v>1</v>
+      </c>
+      <c r="F62" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G62" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H62" s="88"/>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="88" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C63" s="88" t="str">
+        <f t="shared" si="3"/>
+        <v>focus=stop</v>
+      </c>
+      <c r="D63" s="88" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E63" s="88" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F63" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G63" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H63" s="88"/>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="88" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C64" s="88" t="str">
+        <f t="shared" si="3"/>
+        <v>move=stop</v>
+      </c>
+      <c r="D64" s="88" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E64" s="88" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F64" s="88" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G64" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H64" s="88"/>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="88"/>
+      <c r="C65" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>=FALSE</v>
+      </c>
+      <c r="D65" s="88"/>
+      <c r="E65" s="88" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="88"/>
+      <c r="G65" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H65" s="88"/>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="B66" s="88"/>
+      <c r="C66" s="88" t="str">
+        <f t="shared" si="1"/>
+        <v>=FALSE</v>
+      </c>
+      <c r="D66" s="88"/>
+      <c r="E66" s="88" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="88"/>
+      <c r="G66" s="88" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H66" s="88"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2025.05.23  1) 2025.05.22: Retry Connect to NYX after send Reboot CMD for NYX  2) 2025.05.22: Added to press registerBTN in main  3) 2025.05.22: Added to wait until NYX is accessible  4) 2) function must be modified to be accessible to nay object in main
</commit_message>
<xml_diff>
--- a/Command/Command.xlsx
+++ b/Command/Command.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Project\Python\TestTool\Command\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6D2E51-E900-4A5D-ADB1-3A3B8E3207D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ACD261-CBF3-48D4-B92C-BB907CC55E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{79FED000-970D-0E48-B65E-FB5160DD82FF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{79FED000-970D-0E48-B65E-FB5160DD82FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Uncooled" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4868" uniqueCount="1498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4871" uniqueCount="1500">
   <si>
     <r>
       <rPr>
@@ -5767,6 +5767,14 @@
   </si>
   <si>
     <t>Mask 2 Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capture NYX</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -16717,7 +16725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E92AE5-296A-4A53-A69F-D6F31FDFEA61}">
   <dimension ref="B1:T157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A150" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O123" sqref="O123"/>
     </sheetView>
   </sheetViews>
@@ -30402,13 +30410,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E81CA2C-2102-45AC-92BA-FE564D531E29}">
   <sheetPr filterMode="1"/>
-  <dimension ref="B1:N259"/>
+  <dimension ref="B1:N260"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B230" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C59" sqref="C59"/>
+      <selection pane="bottomRight" activeCell="F260" sqref="F260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -34752,6 +34760,22 @@
         <v>696</v>
       </c>
       <c r="G259" s="78"/>
+    </row>
+    <row r="260" spans="2:7">
+      <c r="B260" s="82" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C260" s="83" t="s">
+        <v>1499</v>
+      </c>
+      <c r="D260" s="83" t="s">
+        <v>712</v>
+      </c>
+      <c r="E260" s="84">
+        <v>1</v>
+      </c>
+      <c r="F260" s="83"/>
+      <c r="G260" s="78"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:N259" xr:uid="{3E81CA2C-2102-45AC-92BA-FE564D531E29}">

</xml_diff>